<commit_message>
Working transport parameter update
</commit_message>
<xml_diff>
--- a/input_cost.xlsx
+++ b/input_cost.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27726"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{657FF882-6D6A-4EE1-AAAF-47C3015C00A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BCF42ABD-1443-4385-AC9F-1E95A1672A95}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C96BB67-CA3A-48BB-B057-FD1C3B190336}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1855" yWindow="2016" windowWidth="25390" windowHeight="11612" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="20">
   <si>
     <t>tranSubsector</t>
   </si>
@@ -73,6 +73,12 @@
   </si>
   <si>
     <t>trn_freight_road</t>
+  </si>
+  <si>
+    <t>tag</t>
+  </si>
+  <si>
+    <t>input-cost</t>
   </si>
 </sst>
 </file>
@@ -421,10 +427,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T33"/>
+  <dimension ref="A1:U33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -432,9 +438,10 @@
     <col min="1" max="1" width="32.19921875" customWidth="1"/>
     <col min="2" max="2" width="20.59765625" customWidth="1"/>
     <col min="3" max="3" width="16.09765625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.09765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20">
+    <row r="1" spans="1:21">
       <c r="A1" t="s">
         <v>14</v>
       </c>
@@ -444,59 +451,62 @@
       <c r="C1" t="s">
         <v>3</v>
       </c>
-      <c r="D1">
+      <c r="D1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1">
         <v>2020</v>
       </c>
-      <c r="E1">
+      <c r="F1">
         <v>2025</v>
       </c>
-      <c r="F1">
+      <c r="G1">
         <v>2030</v>
       </c>
-      <c r="G1">
+      <c r="H1">
         <v>2035</v>
       </c>
-      <c r="H1">
+      <c r="I1">
         <v>2040</v>
       </c>
-      <c r="I1">
+      <c r="J1">
         <v>2045</v>
       </c>
-      <c r="J1">
+      <c r="K1">
         <v>2050</v>
       </c>
-      <c r="K1">
+      <c r="L1">
         <v>2055</v>
       </c>
-      <c r="L1">
+      <c r="M1">
         <v>2060</v>
       </c>
-      <c r="M1">
+      <c r="N1">
         <v>2065</v>
       </c>
-      <c r="N1">
+      <c r="O1">
         <v>2070</v>
       </c>
-      <c r="O1">
+      <c r="P1">
         <v>2075</v>
       </c>
-      <c r="P1">
+      <c r="Q1">
         <v>2080</v>
       </c>
-      <c r="Q1">
+      <c r="R1">
         <v>2085</v>
       </c>
-      <c r="R1">
+      <c r="S1">
         <v>2090</v>
       </c>
-      <c r="S1">
+      <c r="T1">
         <v>2095</v>
       </c>
-      <c r="T1">
+      <c r="U1">
         <v>2100</v>
       </c>
     </row>
-    <row r="2" spans="1:20">
+    <row r="2" spans="1:21">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -506,17 +516,17 @@
       <c r="C2" t="s">
         <v>4</v>
       </c>
-      <c r="D2">
+      <c r="D2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2">
         <v>7.2400000000000006E-2</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>7.5399999999999995E-2</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>7.85E-2</v>
-      </c>
-      <c r="G2">
-        <v>8.1500000000000003E-2</v>
       </c>
       <c r="H2">
         <v>8.1500000000000003E-2</v>
@@ -557,8 +567,11 @@
       <c r="T2">
         <v>8.1500000000000003E-2</v>
       </c>
-    </row>
-    <row r="3" spans="1:20">
+      <c r="U2">
+        <v>8.1500000000000003E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -568,17 +581,17 @@
       <c r="C3" t="s">
         <v>5</v>
       </c>
-      <c r="D3">
+      <c r="D3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3">
         <v>7.8600000000000003E-2</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>8.1699999999999995E-2</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <v>8.4699999999999998E-2</v>
-      </c>
-      <c r="G3">
-        <v>8.77E-2</v>
       </c>
       <c r="H3">
         <v>8.77E-2</v>
@@ -619,8 +632,11 @@
       <c r="T3">
         <v>8.77E-2</v>
       </c>
-    </row>
-    <row r="4" spans="1:20">
+      <c r="U3">
+        <v>8.77E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -630,17 +646,17 @@
       <c r="C4" t="s">
         <v>6</v>
       </c>
-      <c r="D4">
+      <c r="D4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4">
         <v>7.6899999999999996E-2</v>
       </c>
-      <c r="E4">
+      <c r="F4">
         <v>0.08</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <v>8.3000000000000004E-2</v>
-      </c>
-      <c r="G4">
-        <v>8.5999999999999993E-2</v>
       </c>
       <c r="H4">
         <v>8.5999999999999993E-2</v>
@@ -681,8 +697,11 @@
       <c r="T4">
         <v>8.5999999999999993E-2</v>
       </c>
-    </row>
-    <row r="5" spans="1:20">
+      <c r="U4">
+        <v>8.5999999999999993E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -692,59 +711,62 @@
       <c r="C5" t="s">
         <v>1</v>
       </c>
-      <c r="D5">
+      <c r="D5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5">
         <v>9.6299999999999997E-2</v>
       </c>
-      <c r="E5">
+      <c r="F5">
         <v>9.35E-2</v>
       </c>
-      <c r="F5">
+      <c r="G5">
         <v>8.6199999999999999E-2</v>
       </c>
-      <c r="G5">
+      <c r="H5">
         <v>7.7600000000000002E-2</v>
       </c>
-      <c r="H5">
+      <c r="I5">
         <v>7.7899999999999997E-2</v>
       </c>
-      <c r="I5">
+      <c r="J5">
         <v>7.7799999999999994E-2</v>
       </c>
-      <c r="J5">
+      <c r="K5">
         <v>7.7499999999999999E-2</v>
       </c>
-      <c r="K5">
+      <c r="L5">
         <v>7.7399999999999997E-2</v>
       </c>
-      <c r="L5">
+      <c r="M5">
         <v>7.7299999999999994E-2</v>
       </c>
-      <c r="M5">
+      <c r="N5">
         <v>7.7200000000000005E-2</v>
       </c>
-      <c r="N5">
+      <c r="O5">
         <v>7.6999999999999999E-2</v>
       </c>
-      <c r="O5">
+      <c r="P5">
         <v>7.6899999999999996E-2</v>
       </c>
-      <c r="P5">
+      <c r="Q5">
         <v>7.6799999999999993E-2</v>
       </c>
-      <c r="Q5">
+      <c r="R5">
         <v>7.6700000000000004E-2</v>
       </c>
-      <c r="R5">
+      <c r="S5">
         <v>7.6499999999999999E-2</v>
       </c>
-      <c r="S5">
+      <c r="T5">
         <v>7.6399999999999996E-2</v>
       </c>
-      <c r="T5">
+      <c r="U5">
         <v>7.6300000000000007E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:20">
+    <row r="6" spans="1:21">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -754,59 +776,62 @@
       <c r="C6" t="s">
         <v>7</v>
       </c>
-      <c r="D6">
+      <c r="D6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6">
         <v>0.10879999999999999</v>
       </c>
-      <c r="E6">
+      <c r="F6">
         <v>0.1031</v>
       </c>
-      <c r="F6">
+      <c r="G6">
         <v>9.4299999999999995E-2</v>
       </c>
-      <c r="G6">
+      <c r="H6">
         <v>8.5400000000000004E-2</v>
       </c>
-      <c r="H6">
+      <c r="I6">
         <v>8.6699999999999999E-2</v>
       </c>
-      <c r="I6">
+      <c r="J6">
         <v>8.8099999999999998E-2</v>
       </c>
-      <c r="J6">
+      <c r="K6">
         <v>8.9599999999999999E-2</v>
       </c>
-      <c r="K6">
+      <c r="L6">
         <v>9.1300000000000006E-2</v>
       </c>
-      <c r="L6">
+      <c r="M6">
         <v>9.2799999999999994E-2</v>
       </c>
-      <c r="M6">
+      <c r="N6">
         <v>9.4200000000000006E-2</v>
       </c>
-      <c r="N6">
+      <c r="O6">
         <v>9.5500000000000002E-2</v>
       </c>
-      <c r="O6">
+      <c r="P6">
         <v>9.6600000000000005E-2</v>
       </c>
-      <c r="P6">
+      <c r="Q6">
         <v>9.7500000000000003E-2</v>
       </c>
-      <c r="Q6">
+      <c r="R6">
         <v>9.8299999999999998E-2</v>
       </c>
-      <c r="R6">
+      <c r="S6">
         <v>9.9000000000000005E-2</v>
       </c>
-      <c r="S6">
+      <c r="T6">
         <v>9.9400000000000002E-2</v>
       </c>
-      <c r="T6">
+      <c r="U6">
         <v>9.9900000000000003E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:20">
+    <row r="7" spans="1:21">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -816,17 +841,17 @@
       <c r="C7" t="s">
         <v>4</v>
       </c>
-      <c r="D7">
+      <c r="D7" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7">
         <v>0.3478</v>
       </c>
-      <c r="E7">
+      <c r="F7">
         <v>0.35489999999999999</v>
       </c>
-      <c r="F7">
+      <c r="G7">
         <v>0.36209999999999998</v>
-      </c>
-      <c r="G7">
-        <v>0.36930000000000002</v>
       </c>
       <c r="H7">
         <v>0.36930000000000002</v>
@@ -867,8 +892,11 @@
       <c r="T7">
         <v>0.36930000000000002</v>
       </c>
-    </row>
-    <row r="8" spans="1:20">
+      <c r="U7">
+        <v>0.36930000000000002</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -878,17 +906,17 @@
       <c r="C8" t="s">
         <v>5</v>
       </c>
-      <c r="D8">
+      <c r="D8" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8">
         <v>0.37119999999999997</v>
       </c>
-      <c r="E8">
+      <c r="F8">
         <v>0.38340000000000002</v>
       </c>
-      <c r="F8">
+      <c r="G8">
         <v>0.39560000000000001</v>
-      </c>
-      <c r="G8">
-        <v>0.4078</v>
       </c>
       <c r="H8">
         <v>0.4078</v>
@@ -929,8 +957,11 @@
       <c r="T8">
         <v>0.4078</v>
       </c>
-    </row>
-    <row r="9" spans="1:20">
+      <c r="U8">
+        <v>0.4078</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -940,59 +971,62 @@
       <c r="C9" t="s">
         <v>1</v>
       </c>
-      <c r="D9">
+      <c r="D9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E9">
         <v>0.38979999999999998</v>
       </c>
-      <c r="E9">
+      <c r="F9">
         <v>0.38629999999999998</v>
       </c>
-      <c r="F9">
+      <c r="G9">
         <v>0.36420000000000002</v>
       </c>
-      <c r="G9">
+      <c r="H9">
         <v>0.33679999999999999</v>
       </c>
-      <c r="H9">
+      <c r="I9">
         <v>0.33779999999999999</v>
       </c>
-      <c r="I9">
+      <c r="J9">
         <v>0.3372</v>
       </c>
-      <c r="J9">
+      <c r="K9">
         <v>0.33579999999999999</v>
       </c>
-      <c r="K9">
+      <c r="L9">
         <v>0.33550000000000002</v>
       </c>
-      <c r="L9">
+      <c r="M9">
         <v>0.33500000000000002</v>
       </c>
-      <c r="M9">
+      <c r="N9">
         <v>0.33450000000000002</v>
       </c>
-      <c r="N9">
+      <c r="O9">
         <v>0.33400000000000002</v>
       </c>
-      <c r="O9">
+      <c r="P9">
         <v>0.33339999999999997</v>
       </c>
-      <c r="P9">
+      <c r="Q9">
         <v>0.33289999999999997</v>
       </c>
-      <c r="Q9">
+      <c r="R9">
         <v>0.33229999999999998</v>
       </c>
-      <c r="R9">
+      <c r="S9">
         <v>0.33179999999999998</v>
       </c>
-      <c r="S9">
+      <c r="T9">
         <v>0.33129999999999998</v>
       </c>
-      <c r="T9">
+      <c r="U9">
         <v>0.33079999999999998</v>
       </c>
     </row>
-    <row r="10" spans="1:20">
+    <row r="10" spans="1:21">
       <c r="A10" t="s">
         <v>15</v>
       </c>
@@ -1002,59 +1036,62 @@
       <c r="C10" t="s">
         <v>7</v>
       </c>
-      <c r="D10">
+      <c r="D10" t="s">
+        <v>19</v>
+      </c>
+      <c r="E10">
         <v>0.3775</v>
       </c>
-      <c r="E10">
+      <c r="F10">
         <v>0.36940000000000001</v>
       </c>
-      <c r="F10">
+      <c r="G10">
         <v>0.35420000000000001</v>
       </c>
-      <c r="G10">
+      <c r="H10">
         <v>0.3296</v>
       </c>
-      <c r="H10">
+      <c r="I10">
         <v>0.3291</v>
       </c>
-      <c r="I10">
+      <c r="J10">
         <v>0.32869999999999999</v>
       </c>
-      <c r="J10">
+      <c r="K10">
         <v>0.33800000000000002</v>
       </c>
-      <c r="K10">
+      <c r="L10">
         <v>0.34250000000000003</v>
       </c>
-      <c r="L10">
+      <c r="M10">
         <v>0.34670000000000001</v>
       </c>
-      <c r="M10">
+      <c r="N10">
         <v>0.35049999999999998</v>
       </c>
-      <c r="N10">
+      <c r="O10">
         <v>0.35389999999999999</v>
       </c>
-      <c r="O10">
+      <c r="P10">
         <v>0.35680000000000001</v>
       </c>
-      <c r="P10">
+      <c r="Q10">
         <v>0.3594</v>
       </c>
-      <c r="Q10">
+      <c r="R10">
         <v>0.3614</v>
       </c>
-      <c r="R10">
+      <c r="S10">
         <v>0.36309999999999998</v>
       </c>
-      <c r="S10">
+      <c r="T10">
         <v>0.36449999999999999</v>
       </c>
-      <c r="T10">
+      <c r="U10">
         <v>0.36559999999999998</v>
       </c>
     </row>
-    <row r="11" spans="1:20">
+    <row r="11" spans="1:21">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -1064,8 +1101,8 @@
       <c r="C11" t="s">
         <v>4</v>
       </c>
-      <c r="D11">
-        <v>1</v>
+      <c r="D11" t="s">
+        <v>19</v>
       </c>
       <c r="E11">
         <v>1</v>
@@ -1115,8 +1152,11 @@
       <c r="T11">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:20">
+      <c r="U11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -1126,8 +1166,8 @@
       <c r="C12" t="s">
         <v>5</v>
       </c>
-      <c r="D12">
-        <v>1</v>
+      <c r="D12" t="s">
+        <v>19</v>
       </c>
       <c r="E12">
         <v>1</v>
@@ -1177,8 +1217,11 @@
       <c r="T12">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:20">
+      <c r="U12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21">
       <c r="A13" t="s">
         <v>15</v>
       </c>
@@ -1188,8 +1231,8 @@
       <c r="C13" t="s">
         <v>6</v>
       </c>
-      <c r="D13">
-        <v>1</v>
+      <c r="D13" t="s">
+        <v>19</v>
       </c>
       <c r="E13">
         <v>1</v>
@@ -1239,8 +1282,11 @@
       <c r="T13">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:20">
+      <c r="U13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -1250,8 +1296,8 @@
       <c r="C14" t="s">
         <v>1</v>
       </c>
-      <c r="D14">
-        <v>1</v>
+      <c r="D14" t="s">
+        <v>19</v>
       </c>
       <c r="E14">
         <v>1</v>
@@ -1301,8 +1347,11 @@
       <c r="T14">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:20">
+      <c r="U14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21">
       <c r="A15" t="s">
         <v>15</v>
       </c>
@@ -1312,8 +1361,8 @@
       <c r="C15" t="s">
         <v>7</v>
       </c>
-      <c r="D15">
-        <v>1</v>
+      <c r="D15" t="s">
+        <v>19</v>
       </c>
       <c r="E15">
         <v>1</v>
@@ -1363,8 +1412,11 @@
       <c r="T15">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:20">
+      <c r="U15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21">
       <c r="A16" t="s">
         <v>16</v>
       </c>
@@ -1374,8 +1426,8 @@
       <c r="C16" t="s">
         <v>4</v>
       </c>
-      <c r="D16">
-        <v>2</v>
+      <c r="D16" t="s">
+        <v>19</v>
       </c>
       <c r="E16">
         <v>2</v>
@@ -1425,8 +1477,11 @@
       <c r="T16">
         <v>2</v>
       </c>
-    </row>
-    <row r="17" spans="1:20">
+      <c r="U16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -1436,8 +1491,8 @@
       <c r="C17" t="s">
         <v>5</v>
       </c>
-      <c r="D17">
-        <v>2</v>
+      <c r="D17" t="s">
+        <v>19</v>
       </c>
       <c r="E17">
         <v>2</v>
@@ -1487,8 +1542,11 @@
       <c r="T17">
         <v>2</v>
       </c>
-    </row>
-    <row r="18" spans="1:20">
+      <c r="U17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -1498,8 +1556,8 @@
       <c r="C18" t="s">
         <v>6</v>
       </c>
-      <c r="D18">
-        <v>2</v>
+      <c r="D18" t="s">
+        <v>19</v>
       </c>
       <c r="E18">
         <v>2</v>
@@ -1549,8 +1607,11 @@
       <c r="T18">
         <v>2</v>
       </c>
-    </row>
-    <row r="19" spans="1:20">
+      <c r="U18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21">
       <c r="A19" t="s">
         <v>16</v>
       </c>
@@ -1560,8 +1621,8 @@
       <c r="C19" t="s">
         <v>1</v>
       </c>
-      <c r="D19">
-        <v>2</v>
+      <c r="D19" t="s">
+        <v>19</v>
       </c>
       <c r="E19">
         <v>2</v>
@@ -1611,8 +1672,11 @@
       <c r="T19">
         <v>2</v>
       </c>
-    </row>
-    <row r="20" spans="1:20">
+      <c r="U19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21">
       <c r="A20" t="s">
         <v>16</v>
       </c>
@@ -1622,8 +1686,8 @@
       <c r="C20" t="s">
         <v>7</v>
       </c>
-      <c r="D20">
-        <v>2</v>
+      <c r="D20" t="s">
+        <v>19</v>
       </c>
       <c r="E20">
         <v>2</v>
@@ -1673,8 +1737,11 @@
       <c r="T20">
         <v>2</v>
       </c>
-    </row>
-    <row r="21" spans="1:20">
+      <c r="U20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21">
       <c r="A21" t="s">
         <v>17</v>
       </c>
@@ -1684,8 +1751,8 @@
       <c r="C21" t="s">
         <v>4</v>
       </c>
-      <c r="D21">
-        <v>3</v>
+      <c r="D21" t="s">
+        <v>19</v>
       </c>
       <c r="E21">
         <v>3</v>
@@ -1735,8 +1802,11 @@
       <c r="T21">
         <v>3</v>
       </c>
-    </row>
-    <row r="22" spans="1:20">
+      <c r="U21">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:21">
       <c r="A22" t="s">
         <v>17</v>
       </c>
@@ -1746,8 +1816,8 @@
       <c r="C22" t="s">
         <v>5</v>
       </c>
-      <c r="D22">
-        <v>3</v>
+      <c r="D22" t="s">
+        <v>19</v>
       </c>
       <c r="E22">
         <v>3</v>
@@ -1797,8 +1867,11 @@
       <c r="T22">
         <v>3</v>
       </c>
-    </row>
-    <row r="23" spans="1:20">
+      <c r="U22">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:21">
       <c r="A23" t="s">
         <v>17</v>
       </c>
@@ -1808,8 +1881,8 @@
       <c r="C23" t="s">
         <v>6</v>
       </c>
-      <c r="D23">
-        <v>3</v>
+      <c r="D23" t="s">
+        <v>19</v>
       </c>
       <c r="E23">
         <v>3</v>
@@ -1859,8 +1932,11 @@
       <c r="T23">
         <v>3</v>
       </c>
-    </row>
-    <row r="24" spans="1:20">
+      <c r="U23">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21">
       <c r="A24" t="s">
         <v>17</v>
       </c>
@@ -1870,8 +1946,8 @@
       <c r="C24" t="s">
         <v>1</v>
       </c>
-      <c r="D24">
-        <v>3</v>
+      <c r="D24" t="s">
+        <v>19</v>
       </c>
       <c r="E24">
         <v>3</v>
@@ -1921,8 +1997,11 @@
       <c r="T24">
         <v>3</v>
       </c>
-    </row>
-    <row r="25" spans="1:20">
+      <c r="U24">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21">
       <c r="A25" t="s">
         <v>17</v>
       </c>
@@ -1932,8 +2011,8 @@
       <c r="C25" t="s">
         <v>7</v>
       </c>
-      <c r="D25">
-        <v>3</v>
+      <c r="D25" t="s">
+        <v>19</v>
       </c>
       <c r="E25">
         <v>3</v>
@@ -1983,8 +2062,11 @@
       <c r="T25">
         <v>3</v>
       </c>
-    </row>
-    <row r="26" spans="1:20">
+      <c r="U25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:21">
       <c r="A26" t="s">
         <v>17</v>
       </c>
@@ -1994,8 +2076,8 @@
       <c r="C26" t="s">
         <v>4</v>
       </c>
-      <c r="D26">
-        <v>4</v>
+      <c r="D26" t="s">
+        <v>19</v>
       </c>
       <c r="E26">
         <v>4</v>
@@ -2045,8 +2127,11 @@
       <c r="T26">
         <v>4</v>
       </c>
-    </row>
-    <row r="27" spans="1:20">
+      <c r="U26">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:21">
       <c r="A27" t="s">
         <v>17</v>
       </c>
@@ -2056,8 +2141,8 @@
       <c r="C27" t="s">
         <v>5</v>
       </c>
-      <c r="D27">
-        <v>4</v>
+      <c r="D27" t="s">
+        <v>19</v>
       </c>
       <c r="E27">
         <v>4</v>
@@ -2107,8 +2192,11 @@
       <c r="T27">
         <v>4</v>
       </c>
-    </row>
-    <row r="28" spans="1:20">
+      <c r="U27">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:21">
       <c r="A28" t="s">
         <v>17</v>
       </c>
@@ -2118,8 +2206,8 @@
       <c r="C28" t="s">
         <v>1</v>
       </c>
-      <c r="D28">
-        <v>4</v>
+      <c r="D28" t="s">
+        <v>19</v>
       </c>
       <c r="E28">
         <v>4</v>
@@ -2169,8 +2257,11 @@
       <c r="T28">
         <v>4</v>
       </c>
-    </row>
-    <row r="29" spans="1:20">
+      <c r="U28">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:21">
       <c r="A29" t="s">
         <v>17</v>
       </c>
@@ -2180,8 +2271,8 @@
       <c r="C29" t="s">
         <v>7</v>
       </c>
-      <c r="D29">
-        <v>4</v>
+      <c r="D29" t="s">
+        <v>19</v>
       </c>
       <c r="E29">
         <v>4</v>
@@ -2231,8 +2322,11 @@
       <c r="T29">
         <v>4</v>
       </c>
-    </row>
-    <row r="30" spans="1:20">
+      <c r="U29">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:21">
       <c r="A30" t="s">
         <v>17</v>
       </c>
@@ -2242,8 +2336,8 @@
       <c r="C30" t="s">
         <v>4</v>
       </c>
-      <c r="D30">
-        <v>5</v>
+      <c r="D30" t="s">
+        <v>19</v>
       </c>
       <c r="E30">
         <v>5</v>
@@ -2293,8 +2387,11 @@
       <c r="T30">
         <v>5</v>
       </c>
-    </row>
-    <row r="31" spans="1:20">
+      <c r="U30">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:21">
       <c r="A31" t="s">
         <v>17</v>
       </c>
@@ -2304,8 +2401,8 @@
       <c r="C31" t="s">
         <v>5</v>
       </c>
-      <c r="D31">
-        <v>5</v>
+      <c r="D31" t="s">
+        <v>19</v>
       </c>
       <c r="E31">
         <v>5</v>
@@ -2355,8 +2452,11 @@
       <c r="T31">
         <v>5</v>
       </c>
-    </row>
-    <row r="32" spans="1:20">
+      <c r="U31">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:21">
       <c r="A32" t="s">
         <v>17</v>
       </c>
@@ -2366,8 +2466,8 @@
       <c r="C32" t="s">
         <v>1</v>
       </c>
-      <c r="D32">
-        <v>5</v>
+      <c r="D32" t="s">
+        <v>19</v>
       </c>
       <c r="E32">
         <v>5</v>
@@ -2417,8 +2517,11 @@
       <c r="T32">
         <v>5</v>
       </c>
-    </row>
-    <row r="33" spans="1:20">
+      <c r="U32">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:21">
       <c r="A33" t="s">
         <v>17</v>
       </c>
@@ -2428,8 +2531,8 @@
       <c r="C33" t="s">
         <v>7</v>
       </c>
-      <c r="D33">
-        <v>5</v>
+      <c r="D33" t="s">
+        <v>19</v>
       </c>
       <c r="E33">
         <v>5</v>
@@ -2477,6 +2580,9 @@
         <v>5</v>
       </c>
       <c r="T33">
+        <v>5</v>
+      </c>
+      <c r="U33">
         <v>5</v>
       </c>
     </row>

</xml_diff>